<commit_message>
Rename gen_accuracy_table.m => perr_overall_stats.m, minor fixes
</commit_message>
<xml_diff>
--- a/matlab/testing/template_overall_stats.xlsx
+++ b/matlab/testing/template_overall_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt\matlab\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0467CA0E-DB28-488E-A477-E054C72227F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959C50D4-166A-4918-AA22-5FEE94D3882C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="480" windowWidth="22068" windowHeight="13716" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="23760" windowHeight="11775" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,11 +119,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -135,6 +135,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,143 +456,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CD2DE5-4D6B-4D56-B426-488F6A7D85F0}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="5"/>
-    <col min="6" max="6" width="8.88671875" style="5"/>
-    <col min="10" max="10" width="8.88671875" style="5"/>
-    <col min="14" max="14" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="4"/>
+    <col min="6" max="6" width="8.85546875" style="4"/>
+    <col min="10" max="10" width="8.85546875" style="4"/>
+    <col min="14" max="14" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="6" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="6" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="1" t="s">
+      <c r="O2" s="6"/>
+      <c r="P2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="Q2" s="7"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11">
+        <v>1.3243453999999999</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added calibration summary to perr_overall_stats.m.  Added so_fixture_all calibrate mode.  Add directory name to Excel output file name so that Excel doesn't have a cow.
</commit_message>
<xml_diff>
--- a/matlab/testing/template_overall_stats.xlsx
+++ b/matlab/testing/template_overall_stats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt\matlab\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959C50D4-166A-4918-AA22-5FEE94D3882C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C159CCFD-9B08-4DFF-961E-1259491F0EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="23760" windowHeight="11775" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="6210" yWindow="5370" windowWidth="21330" windowHeight="7890" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Error stats" sheetId="1" r:id="rId1"/>
+    <sheet name="Cal stats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>Calibration</t>
   </si>
@@ -52,16 +53,52 @@
   </si>
   <si>
     <t>Variant:</t>
+  </si>
+  <si>
+    <t>RMS residue</t>
+  </si>
+  <si>
+    <t>Num points</t>
+  </si>
+  <si>
+    <t>Num invalid</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>nocorrect</t>
+  </si>
+  <si>
+    <t>source fix</t>
+  </si>
+  <si>
+    <t>sf nocorrect</t>
+  </si>
+  <si>
+    <t>Uncorrected (mm)</t>
+  </si>
+  <si>
+    <t>Corrected  (mm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,10 +153,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -129,6 +167,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -138,13 +182,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -459,7 +500,7 @@
   <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="A4" sqref="A4:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,56 +516,64 @@
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="B1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="13"/>
+      <c r="N2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="7" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="7"/>
+      <c r="Q2" s="13"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -580,318 +629,316 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11">
-        <v>1.3243453999999999</v>
-      </c>
-      <c r="M4" s="11"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -910,4 +957,139 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360B3DF7-A665-4647-A7ED-94BE661ED6B4}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add check_poses options.true_initial which initializes the pose solution to the ground truth pose, avoiding convergence problems. Various support for there being no data after discarding invalid poses.  Don't try linear correction calibration if there are too many invalid points (or no valid points). In check_poses(), add summary information by file in 'overall'.  This is printed by the 'files' report.
</commit_message>
<xml_diff>
--- a/matlab/testing/template_overall_stats.xlsx
+++ b/matlab/testing/template_overall_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt\matlab\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C159CCFD-9B08-4DFF-961E-1259491F0EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE8B38D-A4A2-40FB-A73C-66D343D2E390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="5370" windowWidth="21330" windowHeight="7890" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="3192" yWindow="15216" windowWidth="27348" windowHeight="7656" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Error stats" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
   <si>
     <t>Calibration</t>
   </si>
@@ -62,18 +62,6 @@
   </si>
   <si>
     <t>Num invalid</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>nocorrect</t>
-  </si>
-  <si>
-    <t>source fix</t>
-  </si>
-  <si>
-    <t>sf nocorrect</t>
   </si>
   <si>
     <t>Uncorrected (mm)</t>
@@ -115,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -152,12 +140,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -180,6 +177,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -497,51 +497,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CD2DE5-4D6B-4D56-B426-488F6A7D85F0}">
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:Q11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="4"/>
-    <col min="6" max="6" width="8.85546875" style="4"/>
-    <col min="10" max="10" width="8.85546875" style="4"/>
-    <col min="14" max="14" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="10" max="10" width="8.88671875" style="4"/>
+    <col min="14" max="14" width="8.88671875" style="4"/>
+    <col min="18" max="18" width="8.88671875" style="4"/>
+    <col min="22" max="22" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>9</v>
-      </c>
+      <c r="B1" s="11"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
-      <c r="F1" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="F1" s="11"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="J1" s="11"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
-      <c r="N1" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="N1" s="11"/>
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R1" s="11"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
@@ -574,8 +577,24 @@
         <v>4</v>
       </c>
       <c r="Q2" s="13"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="12"/>
+      <c r="T2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="13"/>
+      <c r="V2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="12"/>
+      <c r="X2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="13"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,8 +646,32 @@
       <c r="Q3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -645,16 +688,16 @@
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="R4" s="7"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
+      <c r="V4" s="7"/>
       <c r="W4" s="8"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -671,16 +714,16 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
+      <c r="R5" s="7"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
+      <c r="V5" s="7"/>
       <c r="W5" s="8"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -697,16 +740,16 @@
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
+      <c r="R6" s="7"/>
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
+      <c r="V6" s="7"/>
       <c r="W6" s="8"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -723,16 +766,16 @@
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
+      <c r="R7" s="7"/>
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
+      <c r="V7" s="7"/>
       <c r="W7" s="8"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -749,16 +792,16 @@
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
+      <c r="R8" s="7"/>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
+      <c r="V8" s="7"/>
       <c r="W8" s="8"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -775,16 +818,16 @@
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
+      <c r="R9" s="7"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
+      <c r="V9" s="7"/>
       <c r="W9" s="8"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -801,16 +844,16 @@
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
+      <c r="R10" s="7"/>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
+      <c r="V10" s="7"/>
       <c r="W10" s="8"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -827,16 +870,16 @@
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
+      <c r="R11" s="7"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
+      <c r="V11" s="7"/>
       <c r="W11" s="8"/>
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -853,16 +896,16 @@
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
+      <c r="R12" s="7"/>
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
+      <c r="V12" s="7"/>
       <c r="W12" s="8"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -879,16 +922,16 @@
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
+      <c r="R13" s="7"/>
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
+      <c r="V13" s="7"/>
       <c r="W13" s="8"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -905,16 +948,16 @@
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
+      <c r="R14" s="7"/>
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
+      <c r="V14" s="7"/>
       <c r="W14" s="8"/>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -931,29 +974,35 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+      <c r="R15" s="5"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
+      <c r="V15" s="5"/>
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -964,18 +1013,18 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G12"/>
+      <selection activeCell="A2" sqref="A2:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -989,104 +1038,104 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="9"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="9"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="9"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dump pose solution residue statistics in check_poses.m.  Fixed perr_overall_stats.m to work when there are more than 26 columns.
</commit_message>
<xml_diff>
--- a/matlab/testing/template_overall_stats.xlsx
+++ b/matlab/testing/template_overall_stats.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt\matlab\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE8B38D-A4A2-40FB-A73C-66D343D2E390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57BDFE0A-60D4-4EBA-8A46-3BB34007E4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3192" yWindow="15216" windowWidth="27348" windowHeight="7656" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="4272" yWindow="15624" windowWidth="32064" windowHeight="7752" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Error stats" sheetId="1" r:id="rId1"/>
-    <sheet name="Cal stats" sheetId="2" r:id="rId2"/>
+    <sheet name="Residue stats" sheetId="3" r:id="rId2"/>
+    <sheet name="Cal stats" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="11">
   <si>
     <t>Calibration</t>
   </si>
@@ -74,10 +75,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -154,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -170,18 +172,29 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CD2DE5-4D6B-4D56-B426-488F6A7D85F0}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,89 +525,103 @@
     <col min="14" max="14" width="8.88671875" style="4"/>
     <col min="18" max="18" width="8.88671875" style="4"/>
     <col min="22" max="22" width="8.88671875" style="4"/>
+    <col min="25" max="25" width="8.88671875" customWidth="1"/>
+    <col min="26" max="26" width="8.88671875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="17"/>
+      <c r="N2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13" t="s">
+      <c r="O2" s="15"/>
+      <c r="P2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="11" t="s">
+      <c r="Q2" s="17"/>
+      <c r="R2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="13" t="s">
+      <c r="S2" s="15"/>
+      <c r="T2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="11" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="13" t="s">
+      <c r="W2" s="15"/>
+      <c r="X2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="13"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="17"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,8 +697,20 @@
       <c r="Y3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -696,8 +735,12 @@
       <c r="W4" s="8"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -722,8 +765,12 @@
       <c r="W5" s="8"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -748,8 +795,12 @@
       <c r="W6" s="8"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -774,8 +825,12 @@
       <c r="W7" s="8"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -801,7 +856,7 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -827,7 +882,7 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -853,7 +908,7 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -879,7 +934,7 @@
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -905,7 +960,7 @@
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -931,7 +986,7 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -957,7 +1012,7 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -984,36 +1039,468 @@
       <c r="Y15" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Z1"/>
+  <mergeCells count="21">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8153FEEB-04C1-455B-88DE-623A379C877D}">
+  <dimension ref="A1:Y13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="8.88671875" style="4"/>
+    <col min="11" max="11" width="8.88671875" style="4"/>
+    <col min="14" max="14" width="8.88671875" style="4"/>
+    <col min="17" max="17" width="8.88671875" style="4"/>
+    <col min="20" max="20" width="8.88671875" style="4"/>
+    <col min="23" max="23" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="O2" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="R2" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="U2" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="X2" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360B3DF7-A665-4647-A7ED-94BE661ED6B4}">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>